<commit_message>
negative TC are in progress
</commit_message>
<xml_diff>
--- a/TestDocs/2.TestCases_R4D.xlsx
+++ b/TestDocs/2.TestCases_R4D.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EnyFood\Random4Dinner\TestDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E1EC3B-A954-4EC8-81A9-551914054655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CDD7AA-592A-4C19-9F1C-CB6A732DBAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28515" yWindow="1590" windowWidth="15900" windowHeight="16530" xr2:uid="{D7D6AB6B-2B78-4986-9BF0-0733B85187FE}"/>
+    <workbookView xWindow="20835" yWindow="540" windowWidth="17265" windowHeight="15375" xr2:uid="{D7D6AB6B-2B78-4986-9BF0-0733B85187FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases (positive)" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="66">
   <si>
     <t>ID</t>
   </si>
@@ -235,13 +235,28 @@
   </si>
   <si>
     <t>1. Tap the [Save] button</t>
+  </si>
+  <si>
+    <t>Precondition: 
+1. The app is launched
+2. The "Registration" screen is displayed
+3. Tap the [Google Account] button</t>
+  </si>
+  <si>
+    <t>The "Registration" screen is displayed</t>
+  </si>
+  <si>
+    <t>Title: Checking the displaying of the The "Registration" screen</t>
+  </si>
+  <si>
+    <t>1.Tap [Cancel] button</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,8 +280,14 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -327,8 +348,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -486,11 +519,109 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -513,57 +644,6 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -576,6 +656,102 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -891,23 +1067,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3672E832-2791-4F56-88E1-DB873B50D924}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="41.6640625" customWidth="1"/>
-    <col min="4" max="4" width="55.21875" customWidth="1"/>
+    <col min="3" max="3" width="41.7109375" customWidth="1"/>
+    <col min="4" max="4" width="55.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="12" t="s">
         <v>47</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -917,617 +1093,643 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="20"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="26"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="25"/>
-    </row>
-    <row r="4" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="11">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="15">
         <v>1</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="9">
         <v>1</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="15"/>
-    </row>
-    <row r="5" spans="1:5" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="12"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="16" t="s">
+      <c r="D4" s="19"/>
+    </row>
+    <row r="5" spans="1:5" ht="43.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="17"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="21" t="s">
+      <c r="D5" s="33"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="34" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="13"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="24"/>
-    </row>
-    <row r="8" spans="1:5" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="11">
+    <row r="7" spans="1:5" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="35">
         <v>2</v>
       </c>
-      <c r="B8" s="26">
+      <c r="B7" s="37">
+        <v>2</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="44"/>
+    </row>
+    <row r="8" spans="1:5" s="8" customFormat="1" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="30"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="33"/>
+    </row>
+    <row r="9" spans="1:5" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="36"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="31.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="15">
+        <v>2</v>
+      </c>
+      <c r="B10" s="10">
         <v>1</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C10" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="15"/>
-    </row>
-    <row r="9" spans="1:5" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="12"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="16" t="s">
+      <c r="D10" s="41"/>
+    </row>
+    <row r="11" spans="1:5" ht="43.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="16"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="17"/>
-    </row>
-    <row r="10" spans="1:5" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="13"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="4" t="s">
+      <c r="D11" s="14"/>
+    </row>
+    <row r="12" spans="1:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="17"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D12" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="34.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="11">
+    <row r="13" spans="1:5" ht="34.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="15">
         <v>3</v>
       </c>
-      <c r="B11" s="26">
+      <c r="B13" s="9">
         <v>1</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C13" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="15"/>
-    </row>
-    <row r="12" spans="1:5" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="12"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="16" t="s">
+      <c r="D13" s="19"/>
+    </row>
+    <row r="14" spans="1:5" ht="44.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="16"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="17"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="21" t="s">
+      <c r="D14" s="14"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D15" s="22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="13"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="24"/>
-    </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="18" t="s">
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="17"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="23"/>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
-    </row>
-    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="8" t="s">
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="26"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10"/>
-    </row>
-    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="11">
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="29"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="15">
         <v>4</v>
       </c>
-      <c r="B17" s="26">
+      <c r="B19" s="9">
         <v>1</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C19" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="15"/>
-    </row>
-    <row r="18" spans="1:4" ht="49.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="12"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="16" t="s">
+      <c r="D19" s="19"/>
+    </row>
+    <row r="20" spans="1:4" ht="49.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="16"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="17"/>
-    </row>
-    <row r="19" spans="1:4" ht="49.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="13"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="4" t="s">
+      <c r="D20" s="14"/>
+    </row>
+    <row r="21" spans="1:4" ht="49.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="17"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="8" t="s">
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="10"/>
-    </row>
-    <row r="21" spans="1:4" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="11">
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="29"/>
+    </row>
+    <row r="23" spans="1:4" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="15">
         <v>5</v>
       </c>
-      <c r="B21" s="26">
+      <c r="B23" s="9">
         <v>1</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C23" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="15"/>
-    </row>
-    <row r="22" spans="1:4" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="12"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="16" t="s">
+      <c r="D23" s="19"/>
+    </row>
+    <row r="24" spans="1:4" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="16"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="17"/>
-    </row>
-    <row r="23" spans="1:4" ht="47.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="13"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="4" t="s">
+      <c r="D24" s="14"/>
+    </row>
+    <row r="25" spans="1:4" ht="47.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="17"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D25" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="8" t="s">
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="10"/>
-    </row>
-    <row r="25" spans="1:4" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="11">
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="29"/>
+    </row>
+    <row r="27" spans="1:4" ht="26.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="15">
         <v>6</v>
       </c>
-      <c r="B25" s="26">
+      <c r="B27" s="9">
         <v>1</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C27" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="15"/>
-    </row>
-    <row r="26" spans="1:4" ht="49.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="12"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="16" t="s">
+      <c r="D27" s="19"/>
+    </row>
+    <row r="28" spans="1:4" ht="49.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="16"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="17"/>
-    </row>
-    <row r="27" spans="1:4" ht="41.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="13"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="4" t="s">
+      <c r="D28" s="14"/>
+    </row>
+    <row r="29" spans="1:4" ht="41.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="17"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D29" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="8" t="s">
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="10"/>
-    </row>
-    <row r="29" spans="1:4" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="11">
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="29"/>
+    </row>
+    <row r="31" spans="1:4" ht="26.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="15">
         <v>7</v>
       </c>
-      <c r="B29" s="26">
+      <c r="B31" s="9">
         <v>1</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C31" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="15"/>
-    </row>
-    <row r="30" spans="1:4" ht="49.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="12"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="16" t="s">
+      <c r="D31" s="19"/>
+    </row>
+    <row r="32" spans="1:4" ht="49.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="16"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="17"/>
-    </row>
-    <row r="31" spans="1:4" ht="52.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="13"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="4" t="s">
+      <c r="D32" s="14"/>
+    </row>
+    <row r="33" spans="1:4" ht="52.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="17"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D33" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="18" t="s">
+    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="20"/>
-    </row>
-    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="8" t="s">
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="26"/>
+    </row>
+    <row r="35" spans="1:4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="10"/>
-    </row>
-    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="11">
+      <c r="B35" s="28"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="29"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="15">
         <v>8</v>
       </c>
-      <c r="B34" s="26">
+      <c r="B36" s="9">
         <v>1</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C36" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D34" s="15"/>
-    </row>
-    <row r="35" spans="1:4" ht="49.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="12"/>
-      <c r="B35" s="27"/>
-      <c r="C35" s="16" t="s">
+      <c r="D36" s="19"/>
+    </row>
+    <row r="37" spans="1:4" ht="49.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="16"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D35" s="17"/>
-    </row>
-    <row r="36" spans="1:4" ht="49.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="13"/>
-      <c r="B36" s="28"/>
-      <c r="C36" s="4" t="s">
+      <c r="D37" s="14"/>
+    </row>
+    <row r="38" spans="1:4" ht="49.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="17"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D38" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="19.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="11">
+    <row r="39" spans="1:4" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="15">
         <v>9</v>
       </c>
-      <c r="B37" s="26">
+      <c r="B39" s="9">
         <v>1</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C39" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D37" s="15"/>
-    </row>
-    <row r="38" spans="1:4" ht="50.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="12"/>
-      <c r="B38" s="27"/>
-      <c r="C38" s="16" t="s">
+      <c r="D39" s="19"/>
+    </row>
+    <row r="40" spans="1:4" ht="50.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="16"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D38" s="17"/>
-    </row>
-    <row r="39" spans="1:4" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="13"/>
-      <c r="B39" s="28"/>
-      <c r="C39" s="4" t="s">
+      <c r="D40" s="14"/>
+    </row>
+    <row r="41" spans="1:4" ht="44.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="17"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D41" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="11">
+    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="15">
         <v>10</v>
       </c>
-      <c r="B40" s="26">
+      <c r="B42" s="9">
         <v>1</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C42" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D40" s="15"/>
-    </row>
-    <row r="41" spans="1:4" ht="57.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="12"/>
-      <c r="B41" s="27"/>
-      <c r="C41" s="16" t="s">
+      <c r="D42" s="19"/>
+    </row>
+    <row r="43" spans="1:4" ht="57.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="16"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="17"/>
-    </row>
-    <row r="42" spans="1:4" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="13"/>
-      <c r="B42" s="28"/>
-      <c r="C42" s="4" t="s">
+      <c r="D43" s="14"/>
+    </row>
+    <row r="44" spans="1:4" ht="26.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="17"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D44" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="11">
+    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="15">
         <v>11</v>
       </c>
-      <c r="B43" s="26">
+      <c r="B45" s="9">
         <v>1</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C45" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D43" s="15"/>
-    </row>
-    <row r="44" spans="1:4" ht="52.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="12"/>
-      <c r="B44" s="27"/>
-      <c r="C44" s="16" t="s">
+      <c r="D45" s="19"/>
+    </row>
+    <row r="46" spans="1:4" ht="52.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="16"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="17"/>
-    </row>
-    <row r="45" spans="1:4" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="13"/>
-      <c r="B45" s="28"/>
-      <c r="C45" s="4" t="s">
+      <c r="D46" s="14"/>
+    </row>
+    <row r="47" spans="1:4" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="17"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D47" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="11">
+    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="15">
         <v>12</v>
       </c>
-      <c r="B46" s="26">
+      <c r="B48" s="9">
         <v>1</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="C48" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D46" s="15"/>
-    </row>
-    <row r="47" spans="1:4" ht="64.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="12"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="16" t="s">
+      <c r="D48" s="19"/>
+    </row>
+    <row r="49" spans="1:4" ht="64.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="16"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D47" s="17"/>
-    </row>
-    <row r="48" spans="1:4" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="13"/>
-      <c r="B48" s="28"/>
-      <c r="C48" s="4" t="s">
+      <c r="D49" s="14"/>
+    </row>
+    <row r="50" spans="1:4" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="17"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D50" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="11">
+    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="15">
         <v>13</v>
       </c>
-      <c r="B49" s="26">
+      <c r="B51" s="9">
         <v>1</v>
       </c>
-      <c r="C49" s="14" t="s">
+      <c r="C51" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D49" s="15"/>
-    </row>
-    <row r="50" spans="1:4" ht="64.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="12"/>
-      <c r="B50" s="27"/>
-      <c r="C50" s="16" t="s">
+      <c r="D51" s="19"/>
+    </row>
+    <row r="52" spans="1:4" ht="64.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="16"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D50" s="17"/>
-    </row>
-    <row r="51" spans="1:4" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="13"/>
-      <c r="B51" s="28"/>
-      <c r="C51" s="4" t="s">
+      <c r="D52" s="14"/>
+    </row>
+    <row r="53" spans="1:4" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="17"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D53" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="11">
+    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="15">
         <v>14</v>
       </c>
-      <c r="B52" s="26">
+      <c r="B54" s="9">
         <v>1</v>
       </c>
-      <c r="C52" s="14" t="s">
+      <c r="C54" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D52" s="15"/>
-    </row>
-    <row r="53" spans="1:4" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="12"/>
-      <c r="B53" s="27"/>
-      <c r="C53" s="16" t="s">
+      <c r="D54" s="19"/>
+    </row>
+    <row r="55" spans="1:4" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="16"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D53" s="17"/>
-    </row>
-    <row r="54" spans="1:4" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="13"/>
-      <c r="B54" s="28"/>
-      <c r="C54" s="4" t="s">
+      <c r="D55" s="14"/>
+    </row>
+    <row r="56" spans="1:4" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="17"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D56" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="18" t="s">
+    <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B55" s="19"/>
-      <c r="C55" s="19"/>
-      <c r="D55" s="20"/>
-    </row>
-    <row r="56" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="8" t="s">
+      <c r="B57" s="25"/>
+      <c r="C57" s="25"/>
+      <c r="D57" s="26"/>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="10"/>
-    </row>
-    <row r="57" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="11">
+      <c r="B58" s="28"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="29"/>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="15">
         <v>15</v>
       </c>
-      <c r="B57" s="26">
+      <c r="B59" s="9">
         <v>1</v>
       </c>
-      <c r="C57" s="14" t="s">
+      <c r="C59" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D57" s="15"/>
-    </row>
-    <row r="58" spans="1:4" ht="49.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="12"/>
-      <c r="B58" s="27"/>
-      <c r="C58" s="16" t="s">
+      <c r="D59" s="19"/>
+    </row>
+    <row r="60" spans="1:4" ht="49.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="16"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D58" s="17"/>
-    </row>
-    <row r="59" spans="1:4" ht="49.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="13"/>
-      <c r="B59" s="28"/>
-      <c r="C59" s="4" t="s">
+      <c r="D60" s="14"/>
+    </row>
+    <row r="61" spans="1:4" ht="49.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="17"/>
+      <c r="B61" s="11"/>
+      <c r="C61" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D59" s="5"/>
+      <c r="D61" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="60">
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A8:A10"/>
+  <mergeCells count="62">
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A4:A6"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="A23:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>

</xml_diff>